<commit_message>
12/12 - UI Changes
</commit_message>
<xml_diff>
--- a/public/uploads/excel/product-excel-export.xlsx
+++ b/public/uploads/excel/product-excel-export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Product</t>
   </si>
@@ -36,6 +36,48 @@
   </si>
   <si>
     <t>Created on</t>
+  </si>
+  <si>
+    <t>z-mart</t>
+  </si>
+  <si>
+    <t>Polo</t>
+  </si>
+  <si>
+    <t>Kilogram</t>
+  </si>
+  <si>
+    <t>2nd Dec, 2022</t>
+  </si>
+  <si>
+    <t>T-shirts</t>
+  </si>
+  <si>
+    <t>Armany</t>
+  </si>
+  <si>
+    <t>Piece</t>
+  </si>
+  <si>
+    <t>5th Dec, 2022</t>
+  </si>
+  <si>
+    <t>Product 111</t>
+  </si>
+  <si>
+    <t>Zara</t>
+  </si>
+  <si>
+    <t>Product 222</t>
+  </si>
+  <si>
+    <t>Product 333</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>Meter</t>
   </si>
 </sst>
 </file>
@@ -371,7 +413,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="G1" sqref="G1"/>
@@ -411,6 +453,121 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>9788</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>342</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>85958586</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>46598685</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>53258695</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>

<commit_message>
profilt loss excel file export functionality added
</commit_message>
<xml_diff>
--- a/public/uploads/excel/product-excel-export.xlsx
+++ b/public/uploads/excel/product-excel-export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Product</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>Meter</t>
+  </si>
+  <si>
+    <t>xvd</t>
+  </si>
+  <si>
+    <t>22nd Dec, 2022</t>
+  </si>
+  <si>
+    <t>Armany jeans</t>
+  </si>
+  <si>
+    <t>23rd Dec, 2022</t>
   </si>
 </sst>
 </file>
@@ -413,7 +425,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="G1" sqref="G1"/>
@@ -493,7 +505,7 @@
         <v>13</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -566,6 +578,52 @@
       </c>
       <c r="G6" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>1234</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>7869</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>120</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multi images upload function added
</commit_message>
<xml_diff>
--- a/public/uploads/excel/product-excel-export.xlsx
+++ b/public/uploads/excel/product-excel-export.xlsx
@@ -482,7 +482,7 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -505,7 +505,7 @@
         <v>13</v>
       </c>
       <c r="F3">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>

</xml_diff>